<commit_message>
fix bugs and clean code
</commit_message>
<xml_diff>
--- a/forms/app/chw_monthly_meeting.xlsx
+++ b/forms/app/chw_monthly_meeting.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
   <si>
     <t>type</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t>../inputs/contact/place_id</t>
   </si>
   <si>
     <t>place_name</t>
@@ -1167,7 +1164,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -1201,7 +1198,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1224,7 +1221,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1235,7 +1232,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -1286,10 +1283,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1319,13 +1316,13 @@
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="3"/>
@@ -1355,7 +1352,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1415,15 +1412,15 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>17</v>
@@ -1450,13 +1447,13 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1484,13 +1481,13 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1546,13 +1543,13 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1563,7 +1560,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -1585,16 +1582,16 @@
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -1618,10 +1615,10 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1678,13 +1675,13 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1712,13 +1709,13 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1746,13 +1743,13 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1783,7 +1780,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1843,15 +1840,15 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>17</v>
@@ -1878,23 +1875,23 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -1919,7 +1916,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
@@ -1979,18 +1976,18 @@
         <v>13</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -2014,21 +2011,21 @@
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
@@ -2052,18 +2049,18 @@
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -2088,19 +2085,19 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
@@ -2127,10 +2124,10 @@
         <v>22</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2140,7 +2137,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -2160,13 +2157,13 @@
     </row>
     <row r="45">
       <c r="A45" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2197,7 +2194,7 @@
         <v>37</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -28984,7 +28981,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -29020,35 +29017,35 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="9" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -29074,22 +29071,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -29114,23 +29111,23 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="10">
         <f>NOW()</f>
-        <v>44746.38285</v>
+        <v>44748.70709</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>

</xml_diff>